<commit_message>
improved Comment Builder demo template design.
</commit_message>
<xml_diff>
--- a/src/main/resources/com/jxls/plus/demo/comment_markup_demo.xlsx
+++ b/src/main/resources/com/jxls/plus/demo/comment_markup_demo.xlsx
@@ -22,7 +22,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>leonate</author>
-    <author>Vysochyn, Leonid</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -130,32 +129,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Vysochyn, Leonid:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:image(imgBean="image" lastCell="D12" imageType="JPEG")</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -247,7 +220,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -281,7 +254,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -289,21 +262,21 @@
       <b/>
       <sz val="10.5"/>
       <color theme="2" tint="-0.499984740745262"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="major"/>
@@ -312,21 +285,21 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -334,7 +307,7 @@
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.499984740745262"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -363,7 +336,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Verdana"/>
+      <name val="Georgia"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -523,9 +496,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Aspect">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Civic">
   <a:themeElements>
-    <a:clrScheme name="Aspect">
+    <a:clrScheme name="Civic">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -533,48 +506,48 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="323232"/>
+        <a:srgbClr val="646B86"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E3DED1"/>
+        <a:srgbClr val="C5D1D7"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="F07F09"/>
+        <a:srgbClr val="D16349"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="9F2936"/>
+        <a:srgbClr val="CCB400"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="1B587C"/>
+        <a:srgbClr val="8CADAE"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="4E8542"/>
+        <a:srgbClr val="8C7B70"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="604878"/>
+        <a:srgbClr val="8FB08C"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C19859"/>
+        <a:srgbClr val="D19049"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="6B9F25"/>
+        <a:srgbClr val="00A3D6"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="B26B02"/>
+        <a:srgbClr val="694F07"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Aspect">
+    <a:fontScheme name="Civic">
       <a:majorFont>
-        <a:latin typeface="Verdana"/>
+        <a:latin typeface="Georgia"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="굴림"/>
-        <a:font script="Hans" typeface="微软雅黑"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="돋움"/>
+        <a:font script="Hans" typeface="方正舒体"/>
         <a:font script="Hant" typeface="微軟正黑體"/>
-        <a:font script="Arab" typeface="Tahoma"/>
-        <a:font script="Hebr" typeface="Tahoma"/>
-        <a:font script="Thai" typeface="FreesiaUPC"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -595,24 +568,24 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Verdana"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Verdana"/>
+        <a:latin typeface="Georgia"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="굴림"/>
-        <a:font script="Hans" typeface="微软雅黑"/>
-        <a:font script="Hant" typeface="微軟正黑體"/>
-        <a:font script="Arab" typeface="Tahoma"/>
-        <a:font script="Hebr" typeface="Tahoma"/>
-        <a:font script="Thai" typeface="FreesiaUPC"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐ明朝"/>
+        <a:font script="Hang" typeface="바탕"/>
+        <a:font script="Hans" typeface="方正舒体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
         <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Cans" typeface="Euphemia"/>
@@ -629,78 +602,40 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Verdana"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Aspect">
+    <a:fmtScheme name="Civic">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="65000"/>
-                <a:satMod val="270000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="25000">
-              <a:schemeClr val="phClr">
-                <a:tint val="60000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="29000"/>
-                <a:satMod val="400000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="45000"/>
-                <a:satMod val="155000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="60000">
-              <a:schemeClr val="phClr">
-                <a:shade val="95000"/>
-                <a:satMod val="150000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="87000"/>
-                <a:satMod val="250000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="45000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:satMod val="150000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="42500" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="11429" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+        <a:ln w="20000" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -710,27 +645,18 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="65500" dist="38100" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="50800" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="40000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="65500" dist="38100" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="50800" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="40000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="65500" dist="38100" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="40000"/>
+                <a:alpha val="45000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -738,12 +664,41 @@
             <a:camera prst="orthographicFront" fov="0">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="contrasting" dir="t">
-              <a:rot lat="0" lon="0" rev="12000000"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:lightRig>
           </a:scene3d>
-          <a:sp3d prstMaterial="powder">
-            <a:bevelT h="50800"/>
+          <a:sp3d contourW="9525" prstMaterial="matte">
+            <a:bevelT w="0" h="0"/>
+            <a:contourClr>
+              <a:schemeClr val="phClr">
+                <a:shade val="70000"/>
+                <a:satMod val="105000"/>
+              </a:schemeClr>
+            </a:contourClr>
+          </a:sp3d>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="25400" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="45000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront" fov="0">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="soft" dir="b">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d prstMaterial="dkEdge">
+            <a:bevelT w="63500" h="63500" prst="cross"/>
+            <a:contourClr>
+              <a:schemeClr val="phClr"/>
+            </a:contourClr>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -751,43 +706,33 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="35000"/>
-                <a:satMod val="150000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="45000">
-              <a:schemeClr val="phClr">
-                <a:shade val="68000"/>
-                <a:satMod val="155000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="70000"/>
-                <a:satMod val="175000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
         <a:blipFill>
           <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
             <a:duotone>
               <a:schemeClr val="phClr">
-                <a:shade val="800"/>
-                <a:satMod val="150000"/>
+                <a:shade val="70000"/>
+                <a:satMod val="115000"/>
               </a:schemeClr>
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="150000"/>
+                <a:tint val="85000"/>
               </a:schemeClr>
             </a:duotone>
           </a:blip>
-          <a:tile tx="0" ty="0" sx="75000" sy="75000" flip="none" algn="tl"/>
+          <a:tile tx="0" ty="0" sx="85000" sy="85000" flip="none" algn="tl"/>
+        </a:blipFill>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:duotone>
+              <a:schemeClr val="phClr">
+                <a:shade val="65000"/>
+                <a:satMod val="115000"/>
+              </a:schemeClr>
+              <a:schemeClr val="phClr">
+                <a:tint val="85000"/>
+              </a:schemeClr>
+            </a:duotone>
+          </a:blip>
+          <a:tile tx="0" ty="0" sx="65000" sy="65000" flip="none" algn="tl"/>
         </a:blipFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -805,12 +750,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.296875" customWidth="1"/>
-    <col min="2" max="2" width="14.09765625" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" customWidth="1"/>
-    <col min="4" max="4" width="11.296875" customWidth="1"/>
-    <col min="5" max="5" width="11.09765625" customWidth="1"/>
-    <col min="6" max="6" width="12.296875" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6"/>
@@ -924,7 +867,6 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6"/>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
       <c r="A13" s="15" t="s">
         <v>7</v>

</xml_diff>